<commit_message>
Update documentation following latest version of the package
</commit_message>
<xml_diff>
--- a/docs/templates/banff_dictionary.xlsx
+++ b/docs/templates/banff_dictionary.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="read me" sheetId="1" r:id="rId1"/>
+    <sheet name="ReadMe" sheetId="1" r:id="rId1"/>
     <sheet name="Variables" sheetId="2" r:id="rId2"/>
     <sheet name="Categories" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -353,7 +353,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -362,31 +362,152 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Classification date</t>
+          <t>Data Dictionary</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>...2</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>...3</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>...4</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Authors:</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>R Sapir-Pichhadze, E Gitelman, S El Bouzaidi Tiali, G Fabre, J Laforme</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Aim of the document:</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Provide a standard metadata model for the input dataset in the banffIT package. It describes the format and the constraints the input dataset must follow to be able to run the diagnosis assignement process</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Current version:</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Version 1.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Banff Classification version:</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>2017</t>
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Spreadsheets:</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>ReadMe</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Description of the document aims, version, and content</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Variables</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Metadata of the list of minimum input variables to be present in the input dataset along with the contraints they must follow in order to be able to assign diagnoses of the Banff Classification using the banffIT package. It also contains the metadata of all possible output variables.</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Categories</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Code, label, and description of each categorical variables that should be present in the input dataset and that can be present in the output dataset</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Version history:</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+    </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Versions</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>45352</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>init</t>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Initial version of the data dictionary</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>45415</t>
         </is>
       </c>
     </row>

</xml_diff>